<commit_message>
Updated typos in  xsd diff and error in submission templates
</commit_message>
<xml_diff>
--- a/xsds_preview/xsd_change_highlights.xlsx
+++ b/xsds_preview/xsd_change_highlights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\snowman\maddipatlazb\21\mgg\githubSync\xsds_preview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD723253-1601-4D0A-B07C-43C333A5FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36038425-589F-41BE-B368-087C4E468A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12768" activeTab="1" xr2:uid="{CB1EB4DA-D8ED-498C-8DF2-81B833EF49E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CB1EB4DA-D8ED-498C-8DF2-81B833EF49E7}"/>
   </bookViews>
   <sheets>
     <sheet name="clinvar_public.xsd" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>/ClinVarVariationRelease/VariationArchive/ClassifiedRecord/Classifications/GermlineClassification/ReviewStatus</t>
   </si>
   <si>
-    <t>/ClassifiedRecord/RCVList/RCVAccession/InterpretedConditionList</t>
-  </si>
-  <si>
     <t>/ClinVarVariationRelease/VariationArchive/ClassifiedRecord/RCVList/RCVAccession/ClassifiedConditionList</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
     <t>/ClinVarVariationRelease/VariationArchive/InterpretedRecord/(Genotype|Haplotype)/SimpleAllele/Interpretations/Interpretation</t>
   </si>
   <si>
-    <t>/ClinVarVariationRelease/VariationArchive/InterpretedRecord/(Genotype|Haplotype)/SimpleAllele/Classifications/GermlineClassification</t>
-  </si>
-  <si>
     <t>/ClinVarVariationRelease/VariationArchive/ClassifiedRecord/Classifications/SomaticClinicalImpact/</t>
   </si>
   <si>
@@ -402,10 +396,16 @@
     <t>/ClinVarVariationRelease/VariationArchive/IncludedRecord/Classifications/GermlineClassification</t>
   </si>
   <si>
-    <t>/VariationArchive/IncludedRecord/ReviewStatus</t>
-  </si>
-  <si>
     <t>/ClinVarVariationRelease/VariationArchive/IncludedRecord/Classifications/GermlineClassification/ReviewStatus[text() ='no classification for the single variant']</t>
+  </si>
+  <si>
+    <t>/ClinVarVariationRelease/VariationArchive/InterpretedRecord/RCVList/RCVAccession/InterpretedConditionList</t>
+  </si>
+  <si>
+    <t>/ClinVarVariationRelease/VariationArchive/ClassifiedRecord/(Genotype|Haplotype)/SimpleAllele/Classifications/GermlineClassification</t>
+  </si>
+  <si>
+    <t>/ClinVarVariationRelease/VariationArchive/IncludedRecord/ReviewStatus</t>
   </si>
 </sst>
 </file>
@@ -461,11 +461,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,17 +783,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B2BB7-5F56-41CB-A6FF-156A3AB86FA2}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -808,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -816,7 +815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -824,7 +823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -832,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -840,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -848,7 +847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -856,7 +855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -864,7 +863,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -872,7 +871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -880,7 +879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -888,7 +887,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -896,7 +895,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -904,7 +903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -912,7 +911,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -920,7 +919,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -928,7 +927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -936,7 +935,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -944,7 +943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -952,7 +951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -960,7 +959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -968,7 +967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -976,7 +975,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -984,7 +983,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -992,7 +991,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1017,17 +1016,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CD7A71-E2AC-4DFF-9D43-4C97BA4F3867}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="134.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="134.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="134.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1034,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1059,332 +1058,332 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="B12" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>67</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
         <v>71</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>73</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>75</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>84</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>86</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
         <v>88</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>92</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>94</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>96</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
         <v>98</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>103</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>105</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>107</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>109</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>